<commit_message>
add new code 16/4
</commit_message>
<xml_diff>
--- a/Baseline_result.xlsx
+++ b/Baseline_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungn\OneDrive - Intapp\Documents\1_Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_WORK\baseline-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D454B0F-BC97-4B38-94E6-0C976FCDACD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885BDF87-AD75-4F42-982F-859229ECF218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="14292" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Folder: TGCN/T-GCN/T-GCN-PyTorch:  python main.py --data shenzhen --model_name TGCN --max_epochs 100 --learning_rate 0.0001 --weight_decay 0 --batch_size 32 --hidden_dim 64 --loss mse_with_regularizer --settings supervised --gpus 0 --seq_len 32 --pre_len 7</t>
+  </si>
+  <si>
+    <t>GRU</t>
+  </si>
+  <si>
+    <t>Folder: TGCN/T-GCN/T-GCN-PyTorch:  python main.py --data shenzhen --model_name GRU --max_epochs 100 --learning_rate 0.0001 --weight_decay 0 --batch_size 32 --hidden_dim 64 --loss mse_with_regularizer --settings supervised --gpus 0 --seq_len 32 --pre_len 7</t>
+  </si>
+  <si>
+    <t>GCN</t>
   </si>
 </sst>
 </file>
@@ -396,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +499,389 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1E-4</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>840.8</v>
+      </c>
+      <c r="G3">
+        <v>3376470</v>
+      </c>
+      <c r="H3">
+        <v>1837.5</v>
+      </c>
+      <c r="I3">
+        <v>0.95883828401565496</v>
+      </c>
+      <c r="J3">
+        <v>0.81679999999999997</v>
+      </c>
+      <c r="K3">
+        <v>298655514624</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>694.12</v>
+      </c>
+      <c r="G4">
+        <v>2294786</v>
+      </c>
+      <c r="H4">
+        <v>1514</v>
+      </c>
+      <c r="I4">
+        <v>0.97</v>
+      </c>
+      <c r="J4">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="K4">
+        <v>202978459648</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>613.23</v>
+      </c>
+      <c r="G5">
+        <v>1980323</v>
+      </c>
+      <c r="H5">
+        <v>1407</v>
+      </c>
+      <c r="I5">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J5">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="K5">
+        <v>175163588608</v>
+      </c>
+      <c r="L5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>2E-3</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>623.29999999999995</v>
+      </c>
+      <c r="G6">
+        <v>2049461</v>
+      </c>
+      <c r="H6">
+        <v>1431</v>
+      </c>
+      <c r="I6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J6">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K6">
+        <v>181278982144</v>
+      </c>
+      <c r="L6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>725.98</v>
+      </c>
+      <c r="G7">
+        <v>2251792</v>
+      </c>
+      <c r="H7">
+        <v>1500</v>
+      </c>
+      <c r="I7">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="J7">
+        <v>0.85</v>
+      </c>
+      <c r="K7">
+        <v>199175536640</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>690.74</v>
+      </c>
+      <c r="G8">
+        <v>3438364</v>
+      </c>
+      <c r="H8">
+        <v>1854</v>
+      </c>
+      <c r="I8">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="J8">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K8">
+        <v>3438364</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>625.04999999999995</v>
+      </c>
+      <c r="G9">
+        <v>2184623</v>
+      </c>
+      <c r="H9">
+        <v>1478</v>
+      </c>
+      <c r="I9">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="K9">
+        <v>2184623</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>0.01</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>606.38</v>
+      </c>
+      <c r="G10">
+        <v>2482061</v>
+      </c>
+      <c r="H10">
+        <v>1575</v>
+      </c>
+      <c r="I10">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="J10">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="K10">
+        <v>2482061</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>1E-3</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>1969</v>
+      </c>
+      <c r="G11">
+        <v>22413590</v>
+      </c>
+      <c r="H11">
+        <v>4734</v>
+      </c>
+      <c r="I11">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="K11">
+        <v>22413590</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1E-3</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12">
+        <v>1942</v>
+      </c>
+      <c r="G12">
+        <v>22150196</v>
+      </c>
+      <c r="H12">
+        <v>4706</v>
+      </c>
+      <c r="I12">
+        <v>0.73</v>
+      </c>
+      <c r="J12">
+        <v>0.53</v>
+      </c>
+      <c r="K12">
+        <v>22150196</v>
+      </c>
+      <c r="L12">
+        <v>3000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add new code 18/4
</commit_message>
<xml_diff>
--- a/Baseline_result.xlsx
+++ b/Baseline_result.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_WORK\baseline-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885BDF87-AD75-4F42-982F-859229ECF218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAB30D1-52AC-43F6-85C3-0AE332E8D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2505" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -79,6 +90,21 @@
   </si>
   <si>
     <t>GCN</t>
+  </si>
+  <si>
+    <t>Folder: TGCN/T-GCN/T-GCN-PyTorch:  python main.py --data shenzhen --model_name GCN --max_epochs 100 --learning_rate 0.0001 --weight_decay 0 --batch_size 32 --hidden_dim 64 --loss mse_with_regularizer --settings supervised --gpus 0 --seq_len 32 --pre_len 7</t>
+  </si>
+  <si>
+    <t>STGCN</t>
+  </si>
+  <si>
+    <t>python main.py --enable_cuda True --dataset pemsd7-m --n_his 32 --n_pred 7</t>
+  </si>
+  <si>
+    <t>STALSTM</t>
+  </si>
+  <si>
+    <t>python main.py</t>
   </si>
 </sst>
 </file>
@@ -405,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,6 +869,9 @@
       <c r="L11">
         <v>100</v>
       </c>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -880,6 +909,184 @@
       </c>
       <c r="L12">
         <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>0.01</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>2016</v>
+      </c>
+      <c r="G13">
+        <v>23516632</v>
+      </c>
+      <c r="H13">
+        <v>4849</v>
+      </c>
+      <c r="I13">
+        <v>0.71</v>
+      </c>
+      <c r="J13">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="K13">
+        <v>23516632</v>
+      </c>
+      <c r="L13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>1E-3</v>
+      </c>
+      <c r="F14">
+        <v>707</v>
+      </c>
+      <c r="G14">
+        <f>1969.6^2</f>
+        <v>3879324.1599999997</v>
+      </c>
+      <c r="H14">
+        <v>1969.65</v>
+      </c>
+      <c r="L14">
+        <v>1000</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
+        <v>769.7</v>
+      </c>
+      <c r="G15">
+        <f>2086.3^2</f>
+        <v>4352647.6900000004</v>
+      </c>
+      <c r="H15">
+        <v>2086.3000000000002</v>
+      </c>
+      <c r="L15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>625.49372600000004</v>
+      </c>
+      <c r="G16">
+        <f>1831.15^2</f>
+        <v>3353110.3225000002</v>
+      </c>
+      <c r="H16">
+        <v>1831.15</v>
+      </c>
+      <c r="L16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F17">
+        <v>845.75901599999997</v>
+      </c>
+      <c r="G17">
+        <f>2185^2</f>
+        <v>4774225</v>
+      </c>
+      <c r="H17">
+        <v>2185</v>
+      </c>
+      <c r="L17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>0.05</v>
+      </c>
+      <c r="F18">
+        <v>3356</v>
+      </c>
+      <c r="G18">
+        <v>79586797</v>
+      </c>
+      <c r="H18">
+        <v>4996</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="N18" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>